<commit_message>
add huge improvements on interpolation engine, now no needs to add exact number of points or to many dates and many others things
</commit_message>
<xml_diff>
--- a/dataset/models/input/Common Environment.xlsx
+++ b/dataset/models/input/Common Environment.xlsx
@@ -4,7 +4,7 @@
   <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Summary"/>
@@ -97,7 +97,7 @@
     <t>USD2AMD</t>
   </si>
   <si>
-    <t>EUR2CNY</t>
+    <t/>
   </si>
   <si>
     <t>2022-06-23a</t>
@@ -255,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -357,6 +357,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="1" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
@@ -721,19 +724,19 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="50" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="52" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="50" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="51" width="10.719285714285713" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="53" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="51" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
       <c r="A1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="51">
+      <c r="B1" s="52">
         <v>0.5</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="43" t="s">
         <v>18</v>
       </c>
     </row>
@@ -741,10 +744,10 @@
       <c r="A2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="51">
+      <c r="B2" s="52">
         <v>0.5</v>
       </c>
-      <c r="C2" s="42" t="s">
+      <c r="C2" s="43" t="s">
         <v>18</v>
       </c>
     </row>
@@ -764,9 +767,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="50" width="17.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="51" width="17.005" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="26" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="50" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="51" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="27" width="12.576428571428572" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="26" width="21.862142857142857" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="26" width="19.862142857142857" customWidth="1" bestFit="1"/>
@@ -1793,7 +1796,7 @@
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="6"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="42"/>
+      <c r="C1" s="43"/>
       <c r="D1" s="3"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2821,7 +2824,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2"/>
-      <c r="C2" s="42"/>
+      <c r="C2" s="43"/>
       <c r="D2" s="3"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
@@ -3851,7 +3854,7 @@
       <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="43"/>
       <c r="D3" s="3"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -4881,7 +4884,7 @@
       <c r="B4" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="42"/>
+      <c r="C4" s="43"/>
       <c r="D4" s="3"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -5911,7 +5914,7 @@
       <c r="B5" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="42"/>
+      <c r="C5" s="43"/>
       <c r="D5" s="3"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -6939,7 +6942,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="42"/>
+      <c r="C6" s="43"/>
       <c r="D6" s="3"/>
       <c r="E6" s="30"/>
       <c r="F6" s="17"/>
@@ -7967,7 +7970,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="42"/>
+      <c r="C7" s="43"/>
       <c r="D7" s="3"/>
       <c r="E7" s="30"/>
       <c r="F7" s="17"/>
@@ -8995,7 +8998,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="42"/>
+      <c r="C8" s="43"/>
       <c r="D8" s="3"/>
       <c r="E8" s="30"/>
       <c r="F8" s="17"/>
@@ -10023,7 +10026,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="42"/>
+      <c r="C9" s="43"/>
       <c r="D9" s="3"/>
       <c r="E9" s="30"/>
       <c r="F9" s="17"/>
@@ -11051,7 +11054,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="42"/>
+      <c r="C10" s="43"/>
       <c r="D10" s="3"/>
       <c r="E10" s="30"/>
       <c r="F10" s="17"/>
@@ -12075,9 +12078,9 @@
       <c r="AMJ10" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="43"/>
+      <c r="A11" s="44"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="42"/>
+      <c r="C11" s="43"/>
       <c r="D11" s="3"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -13101,9 +13104,9 @@
       <c r="AMJ11" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="44"/>
+      <c r="A12" s="45"/>
       <c r="B12" s="2"/>
-      <c r="C12" s="42"/>
+      <c r="C12" s="43"/>
       <c r="D12" s="3"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -14129,7 +14132,7 @@
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
       <c r="A13" s="6"/>
       <c r="B13" s="2"/>
-      <c r="C13" s="42"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="3"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -15155,7 +15158,7 @@
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
       <c r="A14" s="6"/>
       <c r="B14" s="2"/>
-      <c r="C14" s="42"/>
+      <c r="C14" s="43"/>
       <c r="D14" s="3"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -16181,7 +16184,7 @@
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
       <c r="A15" s="6"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="42"/>
+      <c r="C15" s="43"/>
       <c r="D15" s="3"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
@@ -17207,7 +17210,7 @@
     <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
       <c r="A16" s="6"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="42"/>
+      <c r="C16" s="43"/>
       <c r="D16" s="3"/>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -18239,10 +18242,10 @@
       <c r="D17" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="E17" s="45" t="s">
+      <c r="E17" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="45" t="s">
+      <c r="F17" s="46" t="s">
         <v>30</v>
       </c>
       <c r="G17" s="1"/>
@@ -19262,14 +19265,14 @@
       <c r="AMG17" s="1"/>
       <c r="AMH17" s="1"/>
       <c r="AMI17" s="1"/>
-      <c r="AMJ17" s="42"/>
+      <c r="AMJ17" s="43"/>
     </row>
     <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
       <c r="A18" s="14" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="46"/>
+      <c r="C18" s="47"/>
       <c r="D18" s="3"/>
       <c r="E18" s="2" t="s">
         <v>31</v>
@@ -20287,21 +20290,21 @@
       <c r="ALZ18" s="1"/>
       <c r="AMA18" s="1"/>
       <c r="AMB18" s="1"/>
-      <c r="AMC18" s="42"/>
-      <c r="AMD18" s="42"/>
-      <c r="AME18" s="42"/>
-      <c r="AMF18" s="42"/>
-      <c r="AMG18" s="42"/>
-      <c r="AMH18" s="42"/>
-      <c r="AMI18" s="42"/>
-      <c r="AMJ18" s="42"/>
+      <c r="AMC18" s="43"/>
+      <c r="AMD18" s="43"/>
+      <c r="AME18" s="43"/>
+      <c r="AMF18" s="43"/>
+      <c r="AMG18" s="43"/>
+      <c r="AMH18" s="43"/>
+      <c r="AMI18" s="43"/>
+      <c r="AMJ18" s="43"/>
     </row>
     <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
       <c r="A19" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="42"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="3"/>
       <c r="E19" s="2" t="s">
         <v>21</v>
@@ -21329,18 +21332,18 @@
       <c r="AMJ19" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="47"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="2">
         <v>0</v>
       </c>
-      <c r="C20" s="46"/>
+      <c r="C20" s="47"/>
       <c r="D20" s="3">
         <v>44927</v>
       </c>
-      <c r="E20" s="48">
+      <c r="E20" s="49">
         <v>25</v>
       </c>
-      <c r="F20" s="49">
+      <c r="F20" s="50">
         <v>10</v>
       </c>
       <c r="G20" s="1"/>
@@ -22353,24 +22356,24 @@
       <c r="ALZ20" s="1"/>
       <c r="AMA20" s="1"/>
       <c r="AMB20" s="1"/>
-      <c r="AMC20" s="42"/>
-      <c r="AMD20" s="42"/>
-      <c r="AME20" s="42"/>
-      <c r="AMF20" s="42"/>
-      <c r="AMG20" s="42"/>
-      <c r="AMH20" s="42"/>
-      <c r="AMI20" s="42"/>
-      <c r="AMJ20" s="42"/>
+      <c r="AMC20" s="43"/>
+      <c r="AMD20" s="43"/>
+      <c r="AME20" s="43"/>
+      <c r="AMF20" s="43"/>
+      <c r="AMG20" s="43"/>
+      <c r="AMH20" s="43"/>
+      <c r="AMI20" s="43"/>
+      <c r="AMJ20" s="43"/>
     </row>
     <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
       <c r="A21" s="6"/>
       <c r="B21" s="2">
         <v>1</v>
       </c>
-      <c r="C21" s="42"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="3"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
+      <c r="E21" s="50"/>
+      <c r="F21" s="50"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -23395,10 +23398,10 @@
       <c r="B22" s="2">
         <v>2</v>
       </c>
-      <c r="C22" s="42"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
+      <c r="E22" s="50"/>
+      <c r="F22" s="50"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -24423,10 +24426,10 @@
       <c r="B23" s="2">
         <v>3</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="49"/>
-      <c r="F23" s="49"/>
+      <c r="E23" s="50"/>
+      <c r="F23" s="50"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -25451,10 +25454,10 @@
       <c r="B24" s="2">
         <v>4</v>
       </c>
-      <c r="C24" s="42"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="49"/>
-      <c r="F24" s="49"/>
+      <c r="E24" s="50"/>
+      <c r="F24" s="50"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
@@ -26479,10 +26482,10 @@
       <c r="B25" s="2">
         <v>5</v>
       </c>
-      <c r="C25" s="42"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="49"/>
-      <c r="F25" s="49"/>
+      <c r="E25" s="50"/>
+      <c r="F25" s="50"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -27507,10 +27510,10 @@
       <c r="B26" s="2">
         <v>6</v>
       </c>
-      <c r="C26" s="42"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="3"/>
-      <c r="E26" s="49"/>
-      <c r="F26" s="49"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -28535,10 +28538,10 @@
       <c r="B27" s="2">
         <v>7</v>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="43"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="49"/>
-      <c r="F27" s="49"/>
+      <c r="E27" s="50"/>
+      <c r="F27" s="50"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
@@ -29563,10 +29566,10 @@
       <c r="B28" s="2">
         <v>8</v>
       </c>
-      <c r="C28" s="42"/>
+      <c r="C28" s="43"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
+      <c r="E28" s="50"/>
+      <c r="F28" s="50"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
@@ -30591,14 +30594,14 @@
       <c r="B29" s="2">
         <v>9</v>
       </c>
-      <c r="C29" s="42"/>
+      <c r="C29" s="43"/>
       <c r="D29" s="3">
         <v>48214</v>
       </c>
-      <c r="E29" s="49">
+      <c r="E29" s="50">
         <v>40</v>
       </c>
-      <c r="F29" s="49">
+      <c r="F29" s="50">
         <v>15</v>
       </c>
       <c r="G29" s="1"/>
@@ -31625,10 +31628,10 @@
       <c r="B30" s="2">
         <v>10</v>
       </c>
-      <c r="C30" s="42"/>
+      <c r="C30" s="43"/>
       <c r="D30" s="3"/>
-      <c r="E30" s="49"/>
-      <c r="F30" s="49"/>
+      <c r="E30" s="50"/>
+      <c r="F30" s="50"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
@@ -32653,7 +32656,7 @@
       <c r="B31" s="2">
         <v>11</v>
       </c>
-      <c r="C31" s="42"/>
+      <c r="C31" s="43"/>
       <c r="D31" s="3"/>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
@@ -33681,7 +33684,7 @@
       <c r="B32" s="2">
         <v>12</v>
       </c>
-      <c r="C32" s="42"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="3"/>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -34709,7 +34712,7 @@
       <c r="B33" s="2">
         <v>13</v>
       </c>
-      <c r="C33" s="42"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="3"/>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
@@ -35737,7 +35740,7 @@
       <c r="B34" s="2">
         <v>14</v>
       </c>
-      <c r="C34" s="42"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="3"/>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
@@ -36765,7 +36768,7 @@
       <c r="B35" s="2">
         <v>15</v>
       </c>
-      <c r="C35" s="42"/>
+      <c r="C35" s="43"/>
       <c r="D35" s="3"/>
       <c r="E35" s="2"/>
       <c r="F35" s="2"/>
@@ -37793,7 +37796,7 @@
       <c r="B36" s="2">
         <v>16</v>
       </c>
-      <c r="C36" s="42"/>
+      <c r="C36" s="43"/>
       <c r="D36" s="3"/>
       <c r="E36" s="2"/>
       <c r="F36" s="2"/>
@@ -38821,7 +38824,7 @@
       <c r="B37" s="2">
         <v>17</v>
       </c>
-      <c r="C37" s="42"/>
+      <c r="C37" s="43"/>
       <c r="D37" s="3"/>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
@@ -39849,7 +39852,7 @@
       <c r="B38" s="2">
         <v>18</v>
       </c>
-      <c r="C38" s="42"/>
+      <c r="C38" s="43"/>
       <c r="D38" s="3"/>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
@@ -40877,7 +40880,7 @@
       <c r="B39" s="2">
         <v>19</v>
       </c>
-      <c r="C39" s="42"/>
+      <c r="C39" s="43"/>
       <c r="D39" s="3"/>
       <c r="E39" s="2"/>
       <c r="F39" s="2"/>
@@ -41905,7 +41908,7 @@
       <c r="B40" s="2">
         <v>20</v>
       </c>
-      <c r="C40" s="42"/>
+      <c r="C40" s="43"/>
       <c r="D40" s="3"/>
       <c r="E40" s="2"/>
       <c r="F40" s="2"/>
@@ -42933,7 +42936,7 @@
       <c r="B41" s="2">
         <v>21</v>
       </c>
-      <c r="C41" s="42"/>
+      <c r="C41" s="43"/>
       <c r="D41" s="3"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -43968,17 +43971,17 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" style="25" width="17.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="39" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="40" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="25" width="8.005" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="27" width="11.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="40" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="39" width="11.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="41" width="12.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="41" width="11.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="40" width="11.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="42" width="12.290714285714287" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="25" width="10.576428571428572" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="25" width="12.43357142857143" customWidth="1" bestFit="1"/>
   </cols>
@@ -44201,7 +44204,7 @@
       <c r="G17" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="35" t="s">
         <v>26</v>
       </c>
       <c r="I17" s="1"/>
@@ -44238,16 +44241,16 @@
         <v>0</v>
       </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="35">
+      <c r="D20" s="36">
         <v>44927</v>
       </c>
-      <c r="E20" s="36">
+      <c r="E20" s="37">
         <v>1.14</v>
       </c>
-      <c r="F20" s="37">
+      <c r="F20" s="38">
         <v>543</v>
       </c>
-      <c r="G20" s="38">
+      <c r="G20" s="39">
         <f>F20/E20</f>
       </c>
       <c r="H20" s="20"/>
@@ -44259,14 +44262,14 @@
         <f>1+B20</f>
       </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="36">
+      <c r="D21" s="36"/>
+      <c r="E21" s="37">
         <v>1.2</v>
       </c>
-      <c r="F21" s="37">
+      <c r="F21" s="38">
         <v>582</v>
       </c>
-      <c r="G21" s="38">
+      <c r="G21" s="39">
         <f>F21/E21</f>
       </c>
       <c r="H21" s="1"/>
@@ -44278,14 +44281,14 @@
         <f>1+B21</f>
       </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="35"/>
-      <c r="E22" s="36">
+      <c r="D22" s="36"/>
+      <c r="E22" s="37">
         <v>1.16</v>
       </c>
-      <c r="F22" s="37">
+      <c r="F22" s="38">
         <v>561</v>
       </c>
-      <c r="G22" s="38">
+      <c r="G22" s="39">
         <f>F22/E22</f>
       </c>
       <c r="H22" s="1"/>
@@ -44297,14 +44300,14 @@
         <f>1+B22</f>
       </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="36">
+      <c r="D23" s="36"/>
+      <c r="E23" s="37">
         <v>1.14</v>
       </c>
-      <c r="F23" s="37">
+      <c r="F23" s="38">
         <v>553</v>
       </c>
-      <c r="G23" s="38">
+      <c r="G23" s="39">
         <f>F23/E23</f>
       </c>
       <c r="H23" s="1"/>
@@ -44316,14 +44319,14 @@
         <f>1+B23</f>
       </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="35"/>
-      <c r="E24" s="36">
+      <c r="D24" s="36"/>
+      <c r="E24" s="37">
         <v>1.12</v>
       </c>
-      <c r="F24" s="37">
+      <c r="F24" s="38">
         <v>530</v>
       </c>
-      <c r="G24" s="38">
+      <c r="G24" s="39">
         <f>F24/E24</f>
       </c>
       <c r="H24" s="1"/>
@@ -44335,14 +44338,14 @@
         <f>1+B24</f>
       </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="35"/>
-      <c r="E25" s="36">
+      <c r="D25" s="36"/>
+      <c r="E25" s="37">
         <v>1.12</v>
       </c>
-      <c r="F25" s="37">
+      <c r="F25" s="38">
         <v>527</v>
       </c>
-      <c r="G25" s="38">
+      <c r="G25" s="39">
         <f>F25/E25</f>
       </c>
       <c r="H25" s="1"/>
@@ -44354,14 +44357,14 @@
         <f>1+B25</f>
       </c>
       <c r="C26" s="1"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="36">
+      <c r="D26" s="36"/>
+      <c r="E26" s="37">
         <v>1.12</v>
       </c>
-      <c r="F26" s="37">
+      <c r="F26" s="38">
         <v>554</v>
       </c>
-      <c r="G26" s="38">
+      <c r="G26" s="39">
         <f>F26/E26</f>
       </c>
       <c r="H26" s="1"/>
@@ -44373,14 +44376,14 @@
         <f>1+B26</f>
       </c>
       <c r="C27" s="1"/>
-      <c r="D27" s="35"/>
-      <c r="E27" s="36">
+      <c r="D27" s="36"/>
+      <c r="E27" s="37">
         <v>1.22</v>
       </c>
-      <c r="F27" s="37">
+      <c r="F27" s="38">
         <v>630</v>
       </c>
-      <c r="G27" s="38">
+      <c r="G27" s="39">
         <f>F27/E27</f>
       </c>
       <c r="H27" s="1"/>
@@ -44392,14 +44395,14 @@
         <f>1+B27</f>
       </c>
       <c r="C28" s="1"/>
-      <c r="D28" s="35"/>
-      <c r="E28" s="36">
+      <c r="D28" s="36"/>
+      <c r="E28" s="37">
         <v>1.18</v>
       </c>
-      <c r="F28" s="37">
+      <c r="F28" s="38">
         <v>585</v>
       </c>
-      <c r="G28" s="38">
+      <c r="G28" s="39">
         <f>F28/E28</f>
       </c>
       <c r="H28" s="1"/>
@@ -44411,16 +44414,16 @@
         <f>1+B28</f>
       </c>
       <c r="C29" s="1"/>
-      <c r="D29" s="35">
+      <c r="D29" s="36">
         <v>48214</v>
       </c>
-      <c r="E29" s="36">
+      <c r="E29" s="37">
         <v>1.13</v>
       </c>
-      <c r="F29" s="37">
+      <c r="F29" s="38">
         <v>540</v>
       </c>
-      <c r="G29" s="38">
+      <c r="G29" s="39">
         <f>F29/E29</f>
       </c>
       <c r="H29" s="20"/>
@@ -44432,14 +44435,14 @@
         <f>1+B29</f>
       </c>
       <c r="C30" s="1"/>
-      <c r="D30" s="35"/>
-      <c r="E30" s="36">
+      <c r="D30" s="36"/>
+      <c r="E30" s="37">
         <v>1.04</v>
       </c>
-      <c r="F30" s="37">
+      <c r="F30" s="38">
         <v>425</v>
       </c>
-      <c r="G30" s="38">
+      <c r="G30" s="39">
         <f>F30/E30</f>
       </c>
       <c r="H30" s="1"/>
@@ -44600,7 +44603,7 @@
   </sheetPr>
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>